<commit_message>
data: update quiz and shape section json data
</commit_message>
<xml_diff>
--- a/data/motif.xlsx
+++ b/data/motif.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yiqiling/Documents/GitHub/bronze-clocks/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A50C2C10-703C-ED41-87D5-1EF08B4551ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{821C66AD-CCA0-7949-8460-1B2B6B062EE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5080" yWindow="1800" windowWidth="28240" windowHeight="17440" xr2:uid="{5A4EE754-321F-3841-8E6C-3A24EE9B7E47}"/>
+    <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" xr2:uid="{5A4EE754-321F-3841-8E6C-3A24EE9B7E47}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -57,14 +57,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>static/images/越王勾践剑.jpeg</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>static/images/长信宫灯.jpg</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Shang Dynasty</t>
   </si>
   <si>
@@ -88,10 +80,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>static/images/司母戊鼎1.jpg</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Inscriptions</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -123,6 +111,58 @@
   </si>
   <si>
     <t>Auspicious cloud motifs are among the most enduring and meaningful symbols in Chinese culture. In the Han dynasty, cloud motifs were formalized into elegant, swirling scrolls.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>static/images/博山炉2.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>static/images/曾侯乙尊盘.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>static/images/鸢鼎.jpeg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>motif_image_path</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>position_left</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>position_top</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>size_w</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>size_h</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>static/images/饕餮纹.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>static/images/夔龙纹.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>static/images/蟠螭纹.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>static/images/祥云纹.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>static/images/山纹.png</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -169,9 +209,15 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -487,119 +533,409 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D703E85-7B12-724E-9DD0-3D9DB347E206}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="3.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" t="s">
+    <row r="1" spans="1:10">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="2">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G2" s="1">
+        <v>26</v>
+      </c>
+      <c r="H2" s="1">
+        <v>23</v>
+      </c>
+      <c r="I2" s="1">
+        <v>15</v>
+      </c>
+      <c r="J2" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G3" s="1">
+        <v>21</v>
+      </c>
+      <c r="H3" s="1">
+        <v>19</v>
+      </c>
+      <c r="I3" s="1">
+        <v>25</v>
+      </c>
+      <c r="J3" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="1">
         <v>1</v>
       </c>
-      <c r="F1" t="s">
+      <c r="B4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" s="1">
+        <v>23</v>
+      </c>
+      <c r="H4" s="1">
+        <v>17</v>
+      </c>
+      <c r="I4" s="1">
+        <v>20</v>
+      </c>
+      <c r="J4" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="2">
         <v>2</v>
       </c>
-      <c r="G1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="B5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G5" s="1">
+        <v>23</v>
+      </c>
+      <c r="H5" s="1">
+        <v>5</v>
+      </c>
+      <c r="I5" s="1">
+        <v>19</v>
+      </c>
+      <c r="J5" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="1">
+        <v>15</v>
+      </c>
+      <c r="H6" s="1">
+        <v>16</v>
+      </c>
+      <c r="I6" s="1">
+        <v>9</v>
+      </c>
+      <c r="J6" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="1">
+        <v>14</v>
+      </c>
+      <c r="H7" s="1">
+        <v>22</v>
+      </c>
+      <c r="I7" s="1">
+        <v>9</v>
+      </c>
+      <c r="J7" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="1">
+        <v>42</v>
+      </c>
+      <c r="H8" s="1">
+        <v>21</v>
+      </c>
+      <c r="I8" s="1">
         <v>11</v>
       </c>
-      <c r="D2" t="s">
+      <c r="J8" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="1">
+        <v>41</v>
+      </c>
+      <c r="H9" s="1">
+        <v>16</v>
+      </c>
+      <c r="I9" s="1">
+        <v>9</v>
+      </c>
+      <c r="J9" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" s="2">
+        <v>3</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F10" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G10" s="1">
+        <v>30</v>
+      </c>
+      <c r="H10" s="1">
+        <v>16</v>
+      </c>
+      <c r="I10" s="1">
+        <v>3</v>
+      </c>
+      <c r="J10" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="1">
+        <v>28</v>
+      </c>
+      <c r="H11" s="1">
+        <v>14.5</v>
+      </c>
+      <c r="I11" s="1">
+        <v>2</v>
+      </c>
+      <c r="J11" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="1">
+        <v>34</v>
+      </c>
+      <c r="H12" s="1">
+        <v>14.5</v>
+      </c>
+      <c r="I12" s="1">
+        <v>2</v>
+      </c>
+      <c r="J12" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="1">
+        <v>30</v>
+      </c>
+      <c r="H13" s="1">
+        <v>11.5</v>
+      </c>
+      <c r="I13" s="1">
+        <v>5</v>
+      </c>
+      <c r="J13" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G14" s="1">
+        <v>30.5</v>
+      </c>
+      <c r="H14" s="1">
+        <v>14.5</v>
+      </c>
+      <c r="I14" s="1">
+        <v>3</v>
+      </c>
+      <c r="J14" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="1">
+        <v>27</v>
+      </c>
+      <c r="H15" s="1">
+        <v>18</v>
+      </c>
+      <c r="I15" s="1">
         <v>12</v>
       </c>
-      <c r="F2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4">
+      <c r="J15" s="1">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" t="s">
-        <v>22</v>
-      </c>
-      <c r="F5" t="s">
-        <v>23</v>
-      </c>
-      <c r="G5" t="s">
-        <v>6</v>
-      </c>
     </row>
   </sheetData>
+  <mergeCells count="18">
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="B5:B9"/>
+    <mergeCell ref="B10:B15"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="A5:A9"/>
+    <mergeCell ref="A10:A15"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="C10:C15"/>
+    <mergeCell ref="C5:C9"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D5:D9"/>
+    <mergeCell ref="E5:E9"/>
+    <mergeCell ref="F5:F9"/>
+    <mergeCell ref="D10:D13"/>
+    <mergeCell ref="E10:E13"/>
+    <mergeCell ref="F10:F13"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>